<commit_message>
Modifica del file di Profiling
</commit_message>
<xml_diff>
--- a/Profiling/Domande da porre al dataset.xlsx
+++ b/Profiling/Domande da porre al dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\università\MAGISTRALE\Ing.Dati\Homework 5- repo\Web-Scraping-homework5\Profiling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A17801E-FD19-4745-BAC5-8924595FFE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7707ECC9-412E-4FEA-AC04-F6C540BFD786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analisi strutturale" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Analisi Strutturale</t>
   </si>
@@ -89,6 +89,42 @@
   </si>
   <si>
     <t>Suddividiamo per LTD, SPA, SRL, INC, CORP. Etc..</t>
+  </si>
+  <si>
+    <t>Dipendenza</t>
+  </si>
+  <si>
+    <t>Creazione di una metrica di similarità</t>
+  </si>
+  <si>
+    <t>Informazioni geografiche necessarie</t>
+  </si>
+  <si>
+    <t>Info geografiche necessarie</t>
+  </si>
+  <si>
+    <t>Info su produzione necessarie</t>
+  </si>
+  <si>
+    <t>Info su capitale sociale</t>
+  </si>
+  <si>
+    <t>Info su tipologia di capitale</t>
+  </si>
+  <si>
+    <t>Distirubuzione di prodotti per area geografica</t>
+  </si>
+  <si>
+    <t>info geografiche e produzione</t>
+  </si>
+  <si>
+    <t>Distribuzione della tipologia per area geografica</t>
+  </si>
+  <si>
+    <t>Distribuzione della tipologia per prodotto</t>
+  </si>
+  <si>
+    <t>Distribuzione capitale per geografia</t>
   </si>
 </sst>
 </file>
@@ -104,15 +140,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -120,20 +162,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCellId="1" sqref="A2:XFD2 A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,63 +485,84 @@
     <col min="1" max="1" width="51.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.6640625" customWidth="1"/>
     <col min="3" max="3" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -490,10 +570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA48419D-BE9A-456C-BA39-592D18BC00CB}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,63 +581,124 @@
     <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="45.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>